<commit_message>
Updated 2014 database for 2014. 55 cm counts after Bernys Marín Response e-mail. Still pending his response on the 2012 data.
</commit_message>
<xml_diff>
--- a/data/corvina_length_gillnets5_7_2014.xlsx
+++ b/data/corvina_length_gillnets5_7_2014.xlsx
@@ -38,18 +38,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -81,7 +73,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -550,7 +544,7 @@
         <v>55</v>
       </c>
       <c r="B13" s="2">
-        <v>5.3254602713178301</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>